<commit_message>
Use Image Folder and update results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Fall2019/SupervisedLearning/DNN-RS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB57C8E-D0DA-4445-AF7A-0607B27E34C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0713E64B-27FA-674A-91BD-6F5CEC7B6888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55280" yWindow="4500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{55785084-E7D0-9E40-882E-FDFA09181DD6}"/>
+    <workbookView xWindow="1820" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{55785084-E7D0-9E40-882E-FDFA09181DD6}"/>
   </bookViews>
   <sheets>
     <sheet name="UCM" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H23"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,7 +565,7 @@
         <v>14</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -748,7 +748,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D21"/>
+      <selection activeCell="G13" sqref="G13:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,6 +805,15 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>143.42608537000999</v>
+      </c>
+      <c r="C6">
+        <v>8.8832819927011003E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.97174603174603102</v>
+      </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
@@ -816,6 +825,15 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>143.85543215891801</v>
+      </c>
+      <c r="C7">
+        <v>7.8710013302752194E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.97593650793650699</v>
+      </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
@@ -835,17 +853,17 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="e">
+      <c r="B9">
         <f>AVERAGE(B6:B7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" t="e">
+        <v>143.64075876446401</v>
+      </c>
+      <c r="C9">
         <f t="shared" ref="C9:D9" si="0">AVERAGE(C6:C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" s="4" t="e">
+        <v>8.3771416614881605E-2</v>
+      </c>
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.97384126984126906</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -888,27 +906,45 @@
       <c r="A13" t="s">
         <v>5</v>
       </c>
+      <c r="B13">
+        <v>218.71668514295001</v>
+      </c>
+      <c r="C13">
+        <v>4.1701368287886398E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.98869841269841197</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
+      <c r="B14">
+        <v>217.143963020993</v>
+      </c>
+      <c r="C14">
+        <v>3.2198057287765001E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.99060317460317404</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="e">
+      <c r="B16">
         <f>AVERAGE(B13:B14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" t="e">
-        <f t="shared" ref="C16:D16" si="1">AVERAGE(C13:C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>217.93032408197149</v>
+      </c>
+      <c r="C16">
+        <f>AVERAGE(C13:C14)</f>
+        <v>3.6949712787825703E-2</v>
+      </c>
+      <c r="D16" s="4">
+        <f>AVERAGE(D13:D14)</f>
+        <v>0.989650793650793</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -952,11 +988,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C23" t="e">
-        <f t="shared" ref="C23:D23" si="2">AVERAGE(C20:C21)</f>
+        <f t="shared" ref="C23:D23" si="1">AVERAGE(C20:C21)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D23" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>